<commit_message>
feat: rename `Master_Gate_Status` to `ComplianceGate` and `Compliance_Adjusted_Value` to `AdjustedValue` across calculations and tests, and update the net value calculation formula.
</commit_message>
<xml_diff>
--- a/utils/financial_modeling/output/generated_test.xlsx
+++ b/utils/financial_modeling/output/generated_test.xlsx
@@ -168,13 +168,13 @@
     <definedName name="Gate_Oil_Sheen">'11_Calc_Compliance'!$D$18</definedName>
     <definedName name="Gate_Odor">'11_Calc_Compliance'!$D$19</definedName>
     <definedName name="Gate_Foam">'11_Calc_Compliance'!$D$20</definedName>
-    <definedName name="Master_Gate_Status">'11_Calc_Compliance'!$C$24</definedName>
+    <definedName name="ComplianceGate">'11_Calc_Compliance'!$C$24</definedName>
     <definedName name="S1_Value">'12_Calc_Value'!$E$13</definedName>
     <definedName name="S2_Value">'12_Calc_Value'!$E$14</definedName>
     <definedName name="S3_Value">'12_Calc_Value'!$E$15</definedName>
     <definedName name="S4_Value">'12_Calc_Value'!$E$16</definedName>
     <definedName name="Gross_Value">'12_Calc_Value'!$E$18</definedName>
-    <definedName name="Compliance_Adjusted_Value">'12_Calc_Value'!$E$21</definedName>
+    <definedName name="AdjustedValue">'12_Calc_Value'!$E$21</definedName>
     <definedName name="Testing_Cost">'13_Calc_Costs'!$C$19</definedName>
     <definedName name="MC_Expected_NPV">'14_Calc_Sim'!$B$1016</definedName>
     <definedName name="MC_P10">'14_Calc_Sim'!$B$1017</definedName>
@@ -794,8 +794,8 @@
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="tbl_KPIs" displayName="tbl_KPIs" ref="A12:B22" headerRowCount="1">
-  <autoFilter ref="A12:B22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="tbl_KPIs" displayName="tbl_KPIs" ref="A12:B21" headerRowCount="1">
+  <autoFilter ref="A12:B21"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Metric"/>
     <tableColumn id="2" name="Value"/>
@@ -819,8 +819,8 @@
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="tbl_ScenarioBreakdown" displayName="tbl_ScenarioBreakdown" ref="A30:C34" headerRowCount="1">
-  <autoFilter ref="A30:C34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="tbl_ScenarioBreakdown" displayName="tbl_ScenarioBreakdown" ref="A29:C33" headerRowCount="1">
+  <autoFilter ref="A29:C33"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Scenario"/>
     <tableColumn id="2" name="Gated_Value"/>
@@ -831,8 +831,8 @@
 </file>
 
 <file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="tbl_TreatmentKPIs" displayName="tbl_TreatmentKPIs" ref="A42:C50" headerRowCount="1">
-  <autoFilter ref="A42:C50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="31" name="tbl_TreatmentKPIs" displayName="tbl_TreatmentKPIs" ref="A41:C49" headerRowCount="1">
+  <autoFilter ref="A41:C49"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Metric"/>
     <tableColumn id="2" name="Value"/>
@@ -843,8 +843,8 @@
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="tbl_OptionComparison" displayName="tbl_OptionComparison" ref="A58:D64" headerRowCount="1">
-  <autoFilter ref="A58:D64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="32" name="tbl_OptionComparison" displayName="tbl_OptionComparison" ref="A57:D63" headerRowCount="1">
+  <autoFilter ref="A57:D63"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Metric"/>
     <tableColumn id="2" name="Monthly_HRMS"/>
@@ -2111,7 +2111,7 @@
         <is>
           <t>13-variable compliance gates for water release qualification.
 Each gate returns 1 (PASS) or 0 (FAIL) as numeric value.
-Master_Gate_Status = MIN(all gates) - 0 if ANY gate fails.
+ComplianceGate = MIN(all gates) - 0 if ANY gate fails.
 Numeric gates enable: value gating, fractional compliance (future).
 Gate thresholds defined in 5_EnvironmentalDrivers.</t>
         </is>
@@ -2162,16 +2162,16 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Baseline +/- 5%</t>
+          <t>NAFC &lt;= Target</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>within</t>
+          <t>below</t>
         </is>
       </c>
       <c r="D8" s="29">
-        <f>IF(ABS(Stoch_Efficiency-0.2)&lt;0.05,1,0)</f>
+        <f>IF(Final_NAFC&lt;=Target_NAFC,1,0)</f>
         <v/>
       </c>
       <c r="E8">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Toxicity baseline</t>
+          <t>NAFC toxicity target</t>
         </is>
       </c>
     </row>
@@ -2252,7 +2252,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>&gt; 6.5 mg/L</t>
+          <t>&gt;= 6.5 mg/L</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -2261,7 +2261,7 @@
         </is>
       </c>
       <c r="D11" s="29">
-        <f>IF(Env_DO_Typical_Jul&gt;6.5,1,0)</f>
+        <f>IF(Env_DO_Typical_Jul&gt;=6.5,1,0)</f>
         <v/>
       </c>
       <c r="E11">
@@ -2554,7 +2554,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Master_Gate_Status</t>
+          <t>ComplianceGate</t>
         </is>
       </c>
       <c r="B24">
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="B20" s="29">
-        <f>Master_Gate_Status</f>
+        <f>ComplianceGate</f>
         <v/>
       </c>
       <c r="C20">
@@ -2893,11 +2893,11 @@
     <row r="21">
       <c r="A21" s="12" t="inlineStr">
         <is>
-          <t>Compliance_Adjusted_Value</t>
+          <t>AdjustedValue</t>
         </is>
       </c>
       <c r="E21" s="16">
-        <f>Gross_Value*Master_Gate_Status</f>
+        <f>Gross_Value*ComplianceGate</f>
         <v/>
       </c>
     </row>
@@ -2905,7 +2905,7 @@
     <row r="23">
       <c r="A23" s="31" t="inlineStr">
         <is>
-          <t>Note: Compliance_Adjusted_Value = Gross_Value × Master_Gate_Status</t>
+          <t>Note: AdjustedValue = Gross_Value × ComplianceGate</t>
         </is>
       </c>
     </row>
@@ -3368,7 +3368,7 @@
         <v/>
       </c>
       <c r="H10" s="16">
-        <f>Compliance_Adjusted_Value-Testing_Cost</f>
+        <f>Gross_Value-Testing_Cost</f>
         <v/>
       </c>
       <c r="I10" s="28">
@@ -9531,7 +9531,7 @@
         </is>
       </c>
       <c r="B15" s="33">
-        <f>Compliance_Adjusted_Value</f>
+        <f>AdjustedValue</f>
         <v/>
       </c>
       <c r="C15" t="inlineStr">
@@ -9541,7 +9541,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Gross × Master_Gate_Status</t>
+          <t>Gross × ComplianceGate</t>
         </is>
       </c>
     </row>
@@ -9573,7 +9573,7 @@
         </is>
       </c>
       <c r="B17" s="33">
-        <f>Compliance_Adjusted_Value-Testing_Cost</f>
+        <f>AdjustedValue-Testing_Cost</f>
         <v/>
       </c>
       <c r="C17" t="inlineStr">
@@ -9615,7 +9615,7 @@
         </is>
       </c>
       <c r="B19" s="33">
-        <f>(Compliance_Adjusted_Value-Testing_Cost)/Annual_Throughput</f>
+        <f>(AdjustedValue-Testing_Cost)/Annual_Throughput</f>
         <v/>
       </c>
       <c r="C19" t="inlineStr">
@@ -9707,7 +9707,7 @@
         </is>
       </c>
       <c r="B27" s="33">
-        <f>(Compliance_Adjusted_Value-Testing_Cost)/(Testing_Cost/INDEX(TestOpt_Cost,MATCH(Testing_Option,TestOpt_Option,0)))</f>
+        <f>(AdjustedValue-Testing_Cost)/(Testing_Cost/INDEX(TestOpt_Cost,MATCH(Testing_Option,TestOpt_Option,0)))</f>
         <v/>
       </c>
     </row>
@@ -10349,7 +10349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10554,85 +10554,74 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Compliance Gate Status</t>
+          <t>Annual Testing Cost</t>
         </is>
       </c>
       <c r="B19" s="16">
-        <f>IF(Master_Gate_Status=1,"PASS","FAIL")</f>
+        <f>Testing_Cost</f>
         <v/>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Annual Testing Cost</t>
+          <t>Year 1 Gross Value</t>
         </is>
       </c>
       <c r="B20" s="16">
-        <f>Testing_Cost</f>
+        <f>Year1_Gross_Value</f>
         <v/>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Year 1 Gross Value</t>
+          <t>Year 1 Net Value</t>
         </is>
       </c>
       <c r="B21" s="16">
-        <f>Year1_Gross_Value</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Year 1 Net Value</t>
-        </is>
-      </c>
-      <c r="B22" s="16">
         <f>Year1_Net_Value</f>
         <v/>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="6" t="inlineStr">
+    <row r="23">
+      <c r="A23" s="6" t="inlineStr">
         <is>
           <t>Scenario Value Breakdown</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="31.2" customHeight="1">
+      <c r="A24" s="7" t="inlineStr">
+        <is>
+          <t>Description:</t>
+        </is>
+      </c>
+      <c r="B24" s="8" t="inlineStr">
+        <is>
+          <t>Individual scenario contributions to total gated value with gate status.</t>
         </is>
       </c>
     </row>
     <row r="25" ht="31.2" customHeight="1">
       <c r="A25" s="7" t="inlineStr">
         <is>
-          <t>Description:</t>
+          <t>Purpose:</t>
         </is>
       </c>
       <c r="B25" s="8" t="inlineStr">
         <is>
-          <t>Individual scenario contributions to total gated value with gate status.</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="31.2" customHeight="1">
+          <t>Show which value scenarios are captured by the selected testing option</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="124.8" customHeight="1">
       <c r="A26" s="7" t="inlineStr">
         <is>
-          <t>Purpose:</t>
+          <t>Assumptions:</t>
         </is>
       </c>
       <c r="B26" s="8" t="inlineStr">
-        <is>
-          <t>Show which value scenarios are captured by the selected testing option</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" ht="124.8" customHeight="1">
-      <c r="A27" s="7" t="inlineStr">
-        <is>
-          <t>Assumptions:</t>
-        </is>
-      </c>
-      <c r="B27" s="8" t="inlineStr">
         <is>
           <t>- Gate status determined by testing latency vs required response time
 - ENABLED means testing latency allows capturing this value
@@ -10641,145 +10630,145 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="31.2" customHeight="1">
+    <row r="27" ht="31.2" customHeight="1">
+      <c r="A27" s="7" t="inlineStr">
+        <is>
+          <t>Data Source:</t>
+        </is>
+      </c>
+      <c r="B27" s="8" t="inlineStr">
+        <is>
+          <t>Calculated from 8_Calc_Value gating logic and stochastic multipliers</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="15.6" customHeight="1">
       <c r="A28" s="7" t="inlineStr">
         <is>
-          <t>Data Source:</t>
+          <t>Related Tables:</t>
         </is>
       </c>
       <c r="B28" s="8" t="inlineStr">
         <is>
-          <t>Calculated from 8_Calc_Value gating logic and stochastic multipliers</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" ht="15.6" customHeight="1">
-      <c r="A29" s="7" t="inlineStr">
-        <is>
-          <t>Related Tables:</t>
-        </is>
-      </c>
-      <c r="B29" s="8" t="inlineStr">
-        <is>
           <t>tbl_KPIs, tbl_ValueScenarios, tbl_GatedValues</t>
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" s="9" t="inlineStr">
+        <is>
+          <t>Scenario</t>
+        </is>
+      </c>
+      <c r="B29" s="9" t="inlineStr">
+        <is>
+          <t>Gated_Value</t>
+        </is>
+      </c>
+      <c r="C29" s="9" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
     <row r="30">
-      <c r="A30" s="9" t="inlineStr">
-        <is>
-          <t>Scenario</t>
-        </is>
-      </c>
-      <c r="B30" s="9" t="inlineStr">
-        <is>
-          <t>Gated_Value</t>
-        </is>
-      </c>
-      <c r="C30" s="9" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>S1: Season Extension</t>
+        </is>
+      </c>
+      <c r="B30" s="16">
+        <f>S1_Value</f>
+        <v/>
+      </c>
+      <c r="C30">
+        <f>INDEX(Gate_S1,MATCH(Testing_Option,TestOpt_Option,0))</f>
+        <v/>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>S1: Season Extension</t>
+          <t>S2: Intervention Avoidance</t>
         </is>
       </c>
       <c r="B31" s="16">
-        <f>S1_Value</f>
+        <f>S2_Value</f>
         <v/>
       </c>
       <c r="C31">
-        <f>INDEX(Gate_S1,MATCH(Testing_Option,TestOpt_Option,0))</f>
+        <f>INDEX(Gate_S2,MATCH(Testing_Option,TestOpt_Option,0))</f>
         <v/>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>S2: Intervention Avoidance</t>
+          <t>S3: Spatial Routing</t>
         </is>
       </c>
       <c r="B32" s="16">
-        <f>S2_Value</f>
+        <f>S3_Value</f>
         <v/>
       </c>
       <c r="C32">
-        <f>INDEX(Gate_S2,MATCH(Testing_Option,TestOpt_Option,0))</f>
+        <f>INDEX(Gate_S3,MATCH(Testing_Option,TestOpt_Option,0))</f>
         <v/>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>S3: Spatial Routing</t>
+          <t>S4: Early Detection</t>
         </is>
       </c>
       <c r="B33" s="16">
-        <f>S3_Value</f>
+        <f>S4_Value</f>
         <v/>
       </c>
       <c r="C33">
-        <f>INDEX(Gate_S3,MATCH(Testing_Option,TestOpt_Option,0))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>S4: Early Detection</t>
-        </is>
-      </c>
-      <c r="B34" s="16">
-        <f>S4_Value</f>
-        <v/>
-      </c>
-      <c r="C34">
         <f>INDEX(Gate_S4,MATCH(Testing_Option,TestOpt_Option,0))</f>
         <v/>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="6" t="inlineStr">
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
         <is>
           <t>Treatment Kinetics (Kearl 2022)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="31.2" customHeight="1">
+      <c r="A36" s="7" t="inlineStr">
+        <is>
+          <t>Description:</t>
+        </is>
+      </c>
+      <c r="B36" s="8" t="inlineStr">
+        <is>
+          <t>NAFC degradation parameters and Monte Carlo treatment time estimates.</t>
         </is>
       </c>
     </row>
     <row r="37" ht="31.2" customHeight="1">
       <c r="A37" s="7" t="inlineStr">
         <is>
-          <t>Description:</t>
+          <t>Purpose:</t>
         </is>
       </c>
       <c r="B37" s="8" t="inlineStr">
         <is>
-          <t>NAFC degradation parameters and Monte Carlo treatment time estimates.</t>
-        </is>
-      </c>
-    </row>
-    <row r="38" ht="31.2" customHeight="1">
+          <t>Validate that biosensor-enabled treatment achieves regulatory compliance within season</t>
+        </is>
+      </c>
+    </row>
+    <row r="38" ht="124.8" customHeight="1">
       <c r="A38" s="7" t="inlineStr">
         <is>
-          <t>Purpose:</t>
+          <t>Assumptions:</t>
         </is>
       </c>
       <c r="B38" s="8" t="inlineStr">
-        <is>
-          <t>Validate that biosensor-enabled treatment achieves regulatory compliance within season</t>
-        </is>
-      </c>
-    </row>
-    <row r="39" ht="124.8" customHeight="1">
-      <c r="A39" s="7" t="inlineStr">
-        <is>
-          <t>Assumptions:</t>
-        </is>
-      </c>
-      <c r="B39" s="8" t="inlineStr">
         <is>
           <t>- Based on Kearl (2022) first-order kinetics model for NAFC degradation
 - Initial/target NAFC concentrations from site characterization data
@@ -10788,206 +10777,206 @@
         </is>
       </c>
     </row>
+    <row r="39" ht="15.6" customHeight="1">
+      <c r="A39" s="7" t="inlineStr">
+        <is>
+          <t>Data Source:</t>
+        </is>
+      </c>
+      <c r="B39" s="8" t="inlineStr">
+        <is>
+          <t>Kearl (2022) wetland treatment kinetics research</t>
+        </is>
+      </c>
+    </row>
     <row r="40" ht="15.6" customHeight="1">
       <c r="A40" s="7" t="inlineStr">
         <is>
-          <t>Data Source:</t>
+          <t>Related Tables:</t>
         </is>
       </c>
       <c r="B40" s="8" t="inlineStr">
         <is>
-          <t>Kearl (2022) wetland treatment kinetics research</t>
-        </is>
-      </c>
-    </row>
-    <row r="41" ht="15.6" customHeight="1">
-      <c r="A41" s="7" t="inlineStr">
-        <is>
-          <t>Related Tables:</t>
-        </is>
-      </c>
-      <c r="B41" s="8" t="inlineStr">
-        <is>
           <t>tbl_KPIs, tbl_Triangular, tbl_TreatmentKinetics</t>
         </is>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" s="9" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B41" s="9" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C41" s="9" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
     <row r="42">
-      <c r="A42" s="9" t="inlineStr">
-        <is>
-          <t>Metric</t>
-        </is>
-      </c>
-      <c r="B42" s="9" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="C42" s="9" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Initial NAFC Concentration</t>
+        </is>
+      </c>
+      <c r="B42" s="34">
+        <f>Initial_NAFC</f>
+        <v/>
+      </c>
+      <c r="C42">
+        <f>IF(Initial_NAFC&gt;Target_NAFC,"Above Target","At/Below Target")</f>
+        <v/>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Initial NAFC Concentration</t>
+          <t>Target NAFC Concentration</t>
         </is>
       </c>
       <c r="B43" s="34">
-        <f>Initial_NAFC</f>
-        <v/>
-      </c>
-      <c r="C43">
-        <f>IF(Initial_NAFC&gt;Target_NAFC,"Above Target","At/Below Target")</f>
-        <v/>
+        <f>Target_NAFC</f>
+        <v/>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>"-"</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Target NAFC Concentration</t>
-        </is>
-      </c>
-      <c r="B44" s="34">
-        <f>Target_NAFC</f>
-        <v/>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>"-"</t>
-        </is>
+          <t>Days to Regulatory Compliance</t>
+        </is>
+      </c>
+      <c r="B44" s="35">
+        <f>Days_to_Compliance</f>
+        <v/>
+      </c>
+      <c r="C44">
+        <f>Compliance_Status</f>
+        <v/>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Days to Regulatory Compliance</t>
-        </is>
-      </c>
-      <c r="B45" s="35">
-        <f>Days_to_Compliance</f>
+          <t>Circulation Cycles Required</t>
+        </is>
+      </c>
+      <c r="B45" s="29">
+        <f>Circulation_Cycles</f>
         <v/>
       </c>
       <c r="C45">
-        <f>Compliance_Status</f>
+        <f>IF(Circulation_Cycles&lt;=3,"Standard","Extended")</f>
         <v/>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Circulation Cycles Required</t>
-        </is>
-      </c>
-      <c r="B46" s="29">
-        <f>Circulation_Cycles</f>
+          <t>Treatment Efficiency</t>
+        </is>
+      </c>
+      <c r="B46" s="30">
+        <f>Treatment_Efficiency</f>
         <v/>
       </c>
       <c r="C46">
-        <f>IF(Circulation_Cycles&lt;=3,"Standard","Extended")</f>
+        <f>IF(Treatment_Efficiency&gt;0.2,"Good","Low")</f>
         <v/>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Treatment Efficiency</t>
-        </is>
-      </c>
-      <c r="B47" s="30">
-        <f>Treatment_Efficiency</f>
+          <t>MC Expected Days</t>
+        </is>
+      </c>
+      <c r="B47" s="35">
+        <f>MC_Expected_Days</f>
         <v/>
       </c>
       <c r="C47">
-        <f>IF(Treatment_Efficiency&gt;0.2,"Good","Low")</f>
+        <f>IF(MC_Expected_Days&lt;=Season_Length,"Achievable","Risk")</f>
         <v/>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MC Expected Days</t>
+          <t>MC P90 Days (conservative)</t>
         </is>
       </c>
       <c r="B48" s="35">
-        <f>MC_Expected_Days</f>
+        <f>MC_P90_Days</f>
         <v/>
       </c>
       <c r="C48">
-        <f>IF(MC_Expected_Days&lt;=Season_Length,"Achievable","Risk")</f>
+        <f>IF(MC_P90_Days&lt;=Season_Length,"Low Risk","High Risk")</f>
         <v/>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>MC P90 Days (conservative)</t>
-        </is>
-      </c>
-      <c r="B49" s="35">
-        <f>MC_P90_Days</f>
+          <t>MC Prob(Achievable)</t>
+        </is>
+      </c>
+      <c r="B49" s="30">
+        <f>MC_Prob_Achievable</f>
         <v/>
       </c>
       <c r="C49">
-        <f>IF(MC_P90_Days&lt;=Season_Length,"Low Risk","High Risk")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>MC Prob(Achievable)</t>
-        </is>
-      </c>
-      <c r="B50" s="30">
-        <f>MC_Prob_Achievable</f>
-        <v/>
-      </c>
-      <c r="C50">
         <f>IF(MC_Prob_Achievable&gt;=0.9,"High Confidence","Review Required")</f>
         <v/>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" s="6" t="inlineStr">
+    <row r="51">
+      <c r="A51" s="6" t="inlineStr">
         <is>
           <t>Testing Option Comparison</t>
+        </is>
+      </c>
+    </row>
+    <row r="52" ht="31.2" customHeight="1">
+      <c r="A52" s="7" t="inlineStr">
+        <is>
+          <t>Description:</t>
+        </is>
+      </c>
+      <c r="B52" s="8" t="inlineStr">
+        <is>
+          <t>Side-by-side comparison of gate status and value across all testing options.</t>
         </is>
       </c>
     </row>
     <row r="53" ht="31.2" customHeight="1">
       <c r="A53" s="7" t="inlineStr">
         <is>
-          <t>Description:</t>
+          <t>Purpose:</t>
         </is>
       </c>
       <c r="B53" s="8" t="inlineStr">
         <is>
-          <t>Side-by-side comparison of gate status and value across all testing options.</t>
-        </is>
-      </c>
-    </row>
-    <row r="54" ht="31.2" customHeight="1">
+          <t>Demonstrate the value differential between HRMS and biosensor testing approaches</t>
+        </is>
+      </c>
+    </row>
+    <row r="54" ht="78" customHeight="1">
       <c r="A54" s="7" t="inlineStr">
         <is>
-          <t>Purpose:</t>
+          <t>Assumptions:</t>
         </is>
       </c>
       <c r="B54" s="8" t="inlineStr">
-        <is>
-          <t>Demonstrate the value differential between HRMS and biosensor testing approaches</t>
-        </is>
-      </c>
-    </row>
-    <row r="55" ht="78" customHeight="1">
-      <c r="A55" s="7" t="inlineStr">
-        <is>
-          <t>Assumptions:</t>
-        </is>
-      </c>
-      <c r="B55" s="8" t="inlineStr">
         <is>
           <t>- Monthly HRMS: 42-day turnaround, $60K/season
 - Weekly HRMS: 42-day turnaround, $28.6K/season
@@ -10996,56 +10985,78 @@
         </is>
       </c>
     </row>
-    <row r="56" ht="31.2" customHeight="1">
+    <row r="55" ht="31.2" customHeight="1">
+      <c r="A55" s="7" t="inlineStr">
+        <is>
+          <t>Data Source:</t>
+        </is>
+      </c>
+      <c r="B55" s="8" t="inlineStr">
+        <is>
+          <t>Testing cost quotes and operational latency measurements</t>
+        </is>
+      </c>
+    </row>
+    <row r="56" ht="15.6" customHeight="1">
       <c r="A56" s="7" t="inlineStr">
         <is>
-          <t>Data Source:</t>
+          <t>Related Tables:</t>
         </is>
       </c>
       <c r="B56" s="8" t="inlineStr">
         <is>
-          <t>Testing cost quotes and operational latency measurements</t>
-        </is>
-      </c>
-    </row>
-    <row r="57" ht="15.6" customHeight="1">
-      <c r="A57" s="7" t="inlineStr">
-        <is>
-          <t>Related Tables:</t>
-        </is>
-      </c>
-      <c r="B57" s="8" t="inlineStr">
-        <is>
           <t>tbl_KPIs, tbl_TestOptions, tbl_LatencyGating</t>
         </is>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" s="9" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B57" s="9" t="inlineStr">
+        <is>
+          <t>Monthly_HRMS</t>
+        </is>
+      </c>
+      <c r="C57" s="9" t="inlineStr">
+        <is>
+          <t>Weekly_HRMS</t>
+        </is>
+      </c>
+      <c r="D57" s="9" t="inlineStr">
+        <is>
+          <t>Daily_Biosensor</t>
+        </is>
+      </c>
+    </row>
     <row r="58">
-      <c r="A58" s="9" t="inlineStr">
-        <is>
-          <t>Metric</t>
-        </is>
-      </c>
-      <c r="B58" s="9" t="inlineStr">
-        <is>
-          <t>Monthly_HRMS</t>
-        </is>
-      </c>
-      <c r="C58" s="9" t="inlineStr">
-        <is>
-          <t>Weekly_HRMS</t>
-        </is>
-      </c>
-      <c r="D58" s="9" t="inlineStr">
-        <is>
-          <t>Daily_Biosensor</t>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>S1 Gate</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>BLOCKED</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>BLOCKED</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>ENABLED</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>S1 Gate</t>
+          <t>S2 Gate</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -11067,7 +11078,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>S2 Gate</t>
+          <t>S3 Gate</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -11077,7 +11088,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BLOCKED</t>
+          <t>ENABLED</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -11089,7 +11100,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>S3 Gate</t>
+          <t>S4 Gate</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -11099,7 +11110,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ENABLED</t>
+          <t>BLOCKED</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -11111,94 +11122,72 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>S4 Gate</t>
+          <t>Testing Cost/Season</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>BLOCKED</t>
+          <t>$60,000</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>BLOCKED</t>
+          <t>$28,571</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>ENABLED</t>
+          <t>$10,000</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Testing Cost/Season</t>
+          <t>Potential 5-Year NPV</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>$60,000</t>
+          <t>-$29k</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>$28,571</t>
+          <t>$180k</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>$10,000</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>Potential 5-Year NPV</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>-$29k</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>$180k</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
           <t>$1.1M+</t>
         </is>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" s="4" t="inlineStr">
+        <is>
+          <t>Model Health</t>
+        </is>
+      </c>
+    </row>
     <row r="66">
-      <c r="A66" s="4" t="inlineStr">
-        <is>
-          <t>Model Health</t>
-        </is>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Check Status:</t>
+        </is>
+      </c>
+      <c r="B66">
+        <f>IF(COUNTIF('21_Checks'!D:D,"FAIL")=0,"HEALTHY","REVIEW REQUIRED")</f>
+        <v/>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Check Status:</t>
+          <t>Errors Found:</t>
         </is>
       </c>
       <c r="B67">
-        <f>IF(COUNTIF('21_Checks'!D:D,"FAIL")=0,"HEALTHY","REVIEW REQUIRED")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Errors Found:</t>
-        </is>
-      </c>
-      <c r="B68">
         <f>COUNTIF('21_Checks'!D:D,"FAIL")</f>
         <v/>
       </c>
@@ -11208,9 +11197,7 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B57:D57"/>
     <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B29:D29"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B28:D28"/>
@@ -11218,7 +11205,8 @@
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B25:D25"/>
@@ -11226,6 +11214,7 @@
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B52:D52"/>
     <mergeCell ref="B39:D39"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11706,7 +11695,7 @@
         </is>
       </c>
       <c r="D27">
-        <f>IF(Master_Gate_Status=1,"PASS","FAIL")</f>
+        <f>IF(ComplianceGate=1,"PASS","FAIL")</f>
         <v/>
       </c>
     </row>
@@ -11727,7 +11716,7 @@
         </is>
       </c>
       <c r="D28">
-        <f>IF(Compliance_Adjusted_Value&gt;=0,"PASS","FAIL")</f>
+        <f>IF(AdjustedValue&gt;=0,"PASS","FAIL")</f>
         <v/>
       </c>
     </row>

</xml_diff>